<commit_message>
Made synthesizing costs of menu items deterministic
</commit_message>
<xml_diff>
--- a/data/Cafe_Data_20_rows_excel_check.xlsx
+++ b/data/Cafe_Data_20_rows_excel_check.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="56">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t xml:space="preserve">Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cost</t>
   </si>
   <si>
     <t xml:space="preserve">Thu Apr 01 2010 15:15:11 GMT+0200 (Central European Summer Time)</t>
@@ -183,6 +186,9 @@
   </si>
   <si>
     <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total cost = sum (cost * quantity)</t>
   </si>
 </sst>
 </file>
@@ -294,13 +300,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="58.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.43"/>
@@ -310,7 +316,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="6.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -341,16 +347,19 @@
       <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>1</v>
@@ -368,18 +377,18 @@
         <v>61.88</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>1</v>
@@ -397,18 +406,18 @@
         <v>123.75</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>1</v>
@@ -426,18 +435,18 @@
         <v>49.5</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>1</v>
@@ -455,18 +464,18 @@
         <v>61.88</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>1</v>
@@ -484,18 +493,18 @@
         <v>55.69</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>1</v>
@@ -513,18 +522,18 @@
         <v>61.88</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>1</v>
@@ -542,18 +551,18 @@
         <v>49.5</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="0" t="s">
         <v>22</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>21</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>1</v>
@@ -571,18 +580,18 @@
         <v>55.69</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>1</v>
@@ -600,18 +609,18 @@
         <v>74.25</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>1</v>
@@ -629,18 +638,18 @@
         <v>55.69</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>1</v>
@@ -658,18 +667,18 @@
         <v>117.56</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>1</v>
@@ -687,18 +696,18 @@
         <v>142.31</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>1</v>
@@ -716,18 +725,18 @@
         <v>105.19</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>1</v>
@@ -745,18 +754,18 @@
         <v>105.19</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="0" t="s">
         <v>34</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>33</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>2</v>
@@ -774,18 +783,18 @@
         <v>210.38</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>1</v>
@@ -803,18 +812,18 @@
         <v>74.25</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>1</v>
@@ -832,18 +841,18 @@
         <v>61.88</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>2</v>
@@ -861,18 +870,18 @@
         <v>148.5</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>1</v>
@@ -890,18 +899,18 @@
         <v>61.88</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>1</v>
@@ -919,12 +928,12 @@
         <v>105.19</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -932,25 +941,30 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B27" s="0" t="n">
         <f aca="false">SUMPRODUCT(E2:E21, D2:D21) + SUM(F2:F21) - SUM(G2:G21)</f>
         <v>1782.04</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added route and check to find total cost
</commit_message>
<xml_diff>
--- a/data/Cafe_Data_20_rows_excel_check.xlsx
+++ b/data/Cafe_Data_20_rows_excel_check.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="55">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -49,7 +49,7 @@
     <t xml:space="preserve">Category</t>
   </si>
   <si>
-    <t xml:space="preserve">Cost</t>
+    <t xml:space="preserve">Cost (taken from database after synthesizing deterministically)</t>
   </si>
   <si>
     <t xml:space="preserve">Thu Apr 01 2010 15:15:11 GMT+0200 (Central European Summer Time)</t>
@@ -183,9 +183,6 @@
   </si>
   <si>
     <t xml:space="preserve">Total revenue = sum (rate * quantity + tax – discount):</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes</t>
   </si>
   <si>
     <t xml:space="preserve">Total cost = sum (cost * quantity)</t>
@@ -195,8 +192,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -270,7 +268,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -280,6 +278,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -303,7 +305,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -379,6 +381,9 @@
       <c r="I2" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="J2" s="0" t="n">
+        <v>31.56</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
@@ -408,6 +413,9 @@
       <c r="I3" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="J3" s="0" t="n">
+        <v>75.49</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
@@ -437,6 +445,9 @@
       <c r="I4" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="J4" s="0" t="n">
+        <v>19.31</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
@@ -466,6 +477,9 @@
       <c r="I5" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="J5" s="0" t="n">
+        <v>31.56</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
@@ -495,6 +509,9 @@
       <c r="I6" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="J6" s="0" t="n">
+        <v>27.29</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -524,6 +541,9 @@
       <c r="I7" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="J7" s="0" t="n">
+        <v>31.56</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
@@ -553,6 +573,9 @@
       <c r="I8" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="J8" s="0" t="n">
+        <v>19.31</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
@@ -582,6 +605,9 @@
       <c r="I9" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="J9" s="0" t="n">
+        <v>27.29</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
@@ -611,6 +637,9 @@
       <c r="I10" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="J10" s="0" t="n">
+        <v>45.29</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
@@ -640,6 +669,9 @@
       <c r="I11" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="J11" s="0" t="n">
+        <v>27.29</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
@@ -669,6 +701,9 @@
       <c r="I12" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="J12" s="0" t="n">
+        <v>43.5</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
@@ -698,6 +733,9 @@
       <c r="I13" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="J13" s="0" t="n">
+        <v>68.31</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
@@ -727,6 +765,9 @@
       <c r="I14" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="J14" s="0" t="n">
+        <v>31.56</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
@@ -756,6 +797,9 @@
       <c r="I15" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="J15" s="0" t="n">
+        <v>66.27</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
@@ -785,6 +829,9 @@
       <c r="I16" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="J16" s="0" t="n">
+        <v>31.56</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
@@ -814,6 +861,9 @@
       <c r="I17" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="J17" s="0" t="n">
+        <v>45.29</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
@@ -843,6 +893,9 @@
       <c r="I18" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="J18" s="0" t="n">
+        <v>31.56</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
@@ -872,6 +925,9 @@
       <c r="I19" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="J19" s="0" t="n">
+        <v>45.29</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
@@ -901,6 +957,9 @@
       <c r="I20" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="J20" s="0" t="n">
+        <v>31.56</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
@@ -930,6 +989,9 @@
       <c r="I21" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="J21" s="0" t="n">
+        <v>48.39</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
@@ -958,13 +1020,22 @@
         <f aca="false">SUMPRODUCT(E2:E21, D2:D21) + SUM(F2:F21) - SUM(G2:G21)</f>
         <v>1782.04</v>
       </c>
-      <c r="C27" s="0" t="s">
-        <v>54</v>
+      <c r="C27" s="3" t="b">
+        <f aca="false">1782.04=1782.04</f>
+        <v>1</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <f aca="false">SUMPRODUCT(J2:J21, D2:D21)</f>
+        <v>856.09</v>
+      </c>
+      <c r="C28" s="3" t="b">
+        <f aca="false">856.09=856.09</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added API route for total profit (KPI)
</commit_message>
<xml_diff>
--- a/data/Cafe_Data_20_rows_excel_check.xlsx
+++ b/data/Cafe_Data_20_rows_excel_check.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="56">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -186,6 +186,9 @@
   </si>
   <si>
     <t xml:space="preserve">Total cost = sum (cost * quantity)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total profit = sum ((rate - cost - discount) * quantity)</t>
   </si>
 </sst>
 </file>
@@ -302,10 +305,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
+      <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1021,7 +1024,7 @@
         <v>1782.04</v>
       </c>
       <c r="C27" s="3" t="b">
-        <f aca="false">1782.04=1782.04</f>
+        <f aca="false">1782.04=B27</f>
         <v>1</v>
       </c>
     </row>
@@ -1034,7 +1037,20 @@
         <v>856.09</v>
       </c>
       <c r="C28" s="3" t="b">
-        <f aca="false">856.09=856.09</f>
+        <f aca="false">856.09=B28</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <f aca="false">SUMPRODUCT((E2:E21 - J2:J21 - G2:G21) * D2:D21)</f>
+        <v>583.91</v>
+      </c>
+      <c r="C29" s="3" t="b">
+        <f aca="false">583.91=B29</f>
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added API route for profit margin (KPI)
</commit_message>
<xml_diff>
--- a/data/Cafe_Data_20_rows_excel_check.xlsx
+++ b/data/Cafe_Data_20_rows_excel_check.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="57">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -182,13 +182,16 @@
     <t xml:space="preserve">Same result as with SQL</t>
   </si>
   <si>
-    <t xml:space="preserve">Total revenue = sum (rate * quantity + tax – discount):</t>
+    <t xml:space="preserve">Total revenue = sum (rate * quantity + tax – discount)</t>
   </si>
   <si>
     <t xml:space="preserve">Total cost = sum (cost * quantity)</t>
   </si>
   <si>
     <t xml:space="preserve">Total profit = sum ((rate - cost - discount) * quantity)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Profit margin (%) = (Total Profit / Total Revenue) * 100</t>
   </si>
 </sst>
 </file>
@@ -305,16 +308,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
+      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="58.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.32"/>
@@ -1054,6 +1057,19 @@
         <v>1</v>
       </c>
     </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <f aca="false">(B29/B27) * 100</f>
+        <v>32.7663801037014</v>
+      </c>
+      <c r="C30" s="3" t="b">
+        <f aca="false">32.7663801037014=B30</f>
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Checked Sales over time SQL query in Excel
</commit_message>
<xml_diff>
--- a/data/Cafe_Data_20_rows_excel_check.xlsx
+++ b/data/Cafe_Data_20_rows_excel_check.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="58">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -192,6 +192,11 @@
   </si>
   <si>
     <t xml:space="preserve">Profit margin (%) = (Total Profit / Total Revenue) * 100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sales over time, per day = sum (rate * quantity + tax – discount).
+These 20 records are from the same day, so sales over time =
+total revenue.</t>
   </si>
 </sst>
 </file>
@@ -274,7 +279,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -289,6 +294,10 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -308,13 +317,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
+      <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="58.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.11"/>
@@ -324,7 +333,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="6.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.65"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1067,6 +1076,19 @@
       </c>
       <c r="C30" s="3" t="b">
         <f aca="false">32.7663801037014=B30</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <f aca="false">B27</f>
+        <v>1782.04</v>
+      </c>
+      <c r="C31" s="3" t="b">
+        <f aca="false">1782.04=B31</f>
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added API route for top 5 products by revenue
</commit_message>
<xml_diff>
--- a/data/Cafe_Data_20_rows_excel_check.xlsx
+++ b/data/Cafe_Data_20_rows_excel_check.xlsx
@@ -11,6 +11,9 @@
     <sheet name="Cafe_Data_20_rows" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <pivotCaches>
+    <pivotCache cacheId="1" r:id="rId4"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="63">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -49,7 +52,10 @@
     <t xml:space="preserve">Category</t>
   </si>
   <si>
-    <t xml:space="preserve">Cost (taken from database after synthesizing deterministically)</t>
+    <t xml:space="preserve">Cost (from DB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Profit (aggregated)</t>
   </si>
   <si>
     <t xml:space="preserve">Thu Apr 01 2010 15:15:11 GMT+0200 (Central European Summer Time)</t>
@@ -197,6 +203,20 @@
     <t xml:space="preserve">Sales over time, per day = sum (rate * quantity + tax – discount).
 These 20 records are from the same day, so sales over time =
 total revenue.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Top 5 products by profit = Profit grouped by Item Desc.
+Had trouble sorting by sum of profits, so I just wrote the sorting next
+to the pivot table, of the top 5.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- all -</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sum - Profit (aggregated)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Result</t>
   </si>
 </sst>
 </file>
@@ -245,7 +265,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="11">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -253,8 +273,78 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right style="thin"/>
+      <top style="medium"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="medium"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="medium"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="medium"/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="medium"/>
+      <top style="thin"/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -278,8 +368,26 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -300,16 +408,534 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="24" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="12">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Pivot Table Corner" xfId="20"/>
+    <cellStyle name="Pivot Table Value" xfId="21"/>
+    <cellStyle name="Pivot Table Field" xfId="22"/>
+    <cellStyle name="Pivot Table Category" xfId="23"/>
+    <cellStyle name="Pivot Table Title" xfId="24"/>
+    <cellStyle name="Pivot Table Result" xfId="25"/>
   </cellStyles>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" recordCount="20" createdVersion="3">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:K21" sheet="Cafe_Data_20_rows"/>
+  </cacheSource>
+  <cacheFields count="11">
+    <cacheField name="date" numFmtId="0">
+      <sharedItems count="14">
+        <s v="Thu Apr 01 2010 03:20:18 GMT+0200 (Central European Summer Time)"/>
+        <s v="Thu Apr 01 2010 03:29:38 GMT+0200 (Central European Summer Time)"/>
+        <s v="Thu Apr 01 2010 03:29:46 GMT+0200 (Central European Summer Time)"/>
+        <s v="Thu Apr 01 2010 15:15:11 GMT+0200 (Central European Summer Time)"/>
+        <s v="Thu Apr 01 2010 15:17:35 GMT+0200 (Central European Summer Time)"/>
+        <s v="Thu Apr 01 2010 15:19:55 GMT+0200 (Central European Summer Time)"/>
+        <s v="Thu Apr 01 2010 15:21:34 GMT+0200 (Central European Summer Time)"/>
+        <s v="Thu Apr 01 2010 15:36:33 GMT+0200 (Central European Summer Time)"/>
+        <s v="Thu Apr 01 2010 15:42:05 GMT+0200 (Central European Summer Time)"/>
+        <s v="Thu Apr 01 2010 16:02:15 GMT+0200 (Central European Summer Time)"/>
+        <s v="Thu Apr 01 2010 16:02:35 GMT+0200 (Central European Summer Time)"/>
+        <s v="Thu Apr 01 2010 16:21:32 GMT+0200 (Central European Summer Time)"/>
+        <s v="Thu Apr 01 2010 16:53:24 GMT+0200 (Central European Summer Time)"/>
+        <s v="Thu Apr 01 2010 16:54:32 GMT+0200 (Central European Summer Time)"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Bill Number " numFmtId="0">
+      <sharedItems count="14">
+        <s v="G0470115"/>
+        <s v="G0470116"/>
+        <s v="G0470117"/>
+        <s v="G0470118"/>
+        <s v="G0470120"/>
+        <s v="G0470122"/>
+        <s v="G0470127"/>
+        <s v="G0470128"/>
+        <s v="G0470133"/>
+        <s v="G0470139"/>
+        <s v="G0470140"/>
+        <s v="G0470283"/>
+        <s v="G0470284"/>
+        <s v="G0470285"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Item Desc" numFmtId="0">
+      <sharedItems count="10">
+        <s v="BRAZIL BOURBONSANTOS (AULAIT) "/>
+        <s v="CAPPUCCINO                    "/>
+        <s v="COUNTRY LEMONADE              "/>
+        <s v="LEMON ICED TEA                "/>
+        <s v="MASALA CHAI CUTTING           "/>
+        <s v="MIAMI MELONS                  "/>
+        <s v="MONSOON MALABAR (AULAIT)      "/>
+        <s v="MOROCCAN MINT TEA             "/>
+        <s v="QUA  MINERAL WATER(1000ML)    "/>
+        <s v="SUMATRA MANDHELING (REG)      "/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Quantity" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="2" count="2">
+        <n v="1"/>
+        <n v="2"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Rate" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="40" maxValue="115" count="8">
+        <n v="40"/>
+        <n v="45"/>
+        <n v="50"/>
+        <n v="60"/>
+        <n v="85"/>
+        <n v="95"/>
+        <n v="100"/>
+        <n v="115"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Tax" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="9.5" maxValue="40.38" count="10">
+        <n v="9.5"/>
+        <n v="10.69"/>
+        <n v="11.88"/>
+        <n v="14.25"/>
+        <n v="20.19"/>
+        <n v="22.56"/>
+        <n v="23.75"/>
+        <n v="27.31"/>
+        <n v="28.5"/>
+        <n v="40.38"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Discount" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="0" count="1">
+        <n v="0"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Total" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="49.5" maxValue="210.38" count="10">
+        <n v="49.5"/>
+        <n v="55.69"/>
+        <n v="61.88"/>
+        <n v="74.25"/>
+        <n v="105.19"/>
+        <n v="117.56"/>
+        <n v="123.75"/>
+        <n v="142.31"/>
+        <n v="148.5"/>
+        <n v="210.38"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Category" numFmtId="0">
+      <sharedItems count="1">
+        <s v="BEVERAGE"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Cost (from DB)" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="19.31" maxValue="75.49" count="9">
+        <n v="19.31"/>
+        <n v="27.29"/>
+        <n v="31.56"/>
+        <n v="43.5"/>
+        <n v="45.29"/>
+        <n v="48.39"/>
+        <n v="66.27"/>
+        <n v="68.31"/>
+        <n v="75.49"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Profit (aggregated)" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="14.71" maxValue="106.88" count="12">
+        <n v="14.71"/>
+        <n v="17.71"/>
+        <n v="18.44"/>
+        <n v="18.73"/>
+        <n v="20.69"/>
+        <n v="24.51"/>
+        <n v="29.42"/>
+        <n v="36.61"/>
+        <n v="46.69"/>
+        <n v="51.5"/>
+        <n v="53.44"/>
+        <n v="106.88"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="20">
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="8"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="6"/>
+    <x v="0"/>
+    <x v="6"/>
+    <x v="6"/>
+    <x v="0"/>
+    <x v="6"/>
+    <x v="0"/>
+    <x v="8"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="1"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="2"/>
+    <x v="8"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="11"/>
+    <x v="7"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="11"/>
+    <x v="8"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="3"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="3"/>
+    <x v="7"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="12"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="13"/>
+    <x v="7"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="13"/>
+    <x v="9"/>
+    <x v="0"/>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="13"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="7"/>
+    <x v="7"/>
+    <x v="0"/>
+    <x v="7"/>
+    <x v="0"/>
+    <x v="7"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="4"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="5"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="6"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="5"/>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="4"/>
+    <x v="9"/>
+    <x v="0"/>
+    <x v="9"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="11"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="6"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="7"/>
+    <x v="8"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="8"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="8"/>
+    <x v="0"/>
+    <x v="8"/>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <x v="9"/>
+    <x v="8"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="10"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="5"/>
+    <x v="7"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DataPilot1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="Values" useAutoFormatting="0" itemPrintTitles="1" indent="0" outline="0" outlineData="0" compact="0" compactData="0">
+  <location ref="B34:C40" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="11">
+    <pivotField compact="0" showAll="0"/>
+    <pivotField compact="0" showAll="0"/>
+    <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0" outline="0">
+      <items count="10">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" showAll="0"/>
+    <pivotField compact="0" showAll="0"/>
+    <pivotField compact="0" showAll="0"/>
+    <pivotField compact="0" showAll="0"/>
+    <pivotField compact="0" showAll="0"/>
+    <pivotField compact="0" showAll="0"/>
+    <pivotField compact="0" showAll="0"/>
+    <pivotField axis="axisPage" dataField="1" compact="0" showAll="0" countASubtotal="1" defaultSubtotal="0" outline="0">
+      <items count="13">
+        <item h="1" x="0"/>
+        <item h="1" x="1"/>
+        <item h="1" x="2"/>
+        <item h="1" x="3"/>
+        <item h="1" x="4"/>
+        <item h="1" x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item t="countA"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <pageFields count="1">
+    <pageField fld="10" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum - Profit (aggregated)*" fld="10" subtotal="sum" numFmtId="164"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -317,10 +943,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F39" activeCellId="0" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -334,6 +960,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="6.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="17.09"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -367,16 +995,19 @@
       <c r="J1" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>1</v>
@@ -394,21 +1025,25 @@
         <v>61.88</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>31.56</v>
       </c>
+      <c r="K2" s="0" t="n">
+        <f aca="false">(E2-J2-G2) * D2</f>
+        <v>18.44</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>1</v>
@@ -426,21 +1061,25 @@
         <v>123.75</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J3" s="0" t="n">
         <v>75.49</v>
       </c>
+      <c r="K3" s="0" t="n">
+        <f aca="false">(E3-J3-G3) * D3</f>
+        <v>24.51</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>1</v>
@@ -458,21 +1097,25 @@
         <v>49.5</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J4" s="0" t="n">
         <v>19.31</v>
       </c>
+      <c r="K4" s="0" t="n">
+        <f aca="false">(E4-J4-G4) * D4</f>
+        <v>20.69</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>1</v>
@@ -490,21 +1133,25 @@
         <v>61.88</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J5" s="0" t="n">
         <v>31.56</v>
       </c>
+      <c r="K5" s="0" t="n">
+        <f aca="false">(E5-J5-G5) * D5</f>
+        <v>18.44</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>1</v>
@@ -522,21 +1169,25 @@
         <v>55.69</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J6" s="0" t="n">
         <v>27.29</v>
       </c>
+      <c r="K6" s="0" t="n">
+        <f aca="false">(E6-J6-G6) * D6</f>
+        <v>17.71</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>1</v>
@@ -554,21 +1205,25 @@
         <v>61.88</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J7" s="0" t="n">
         <v>31.56</v>
       </c>
+      <c r="K7" s="0" t="n">
+        <f aca="false">(E7-J7-G7) * D7</f>
+        <v>18.44</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>1</v>
@@ -586,21 +1241,25 @@
         <v>49.5</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J8" s="0" t="n">
         <v>19.31</v>
       </c>
+      <c r="K8" s="0" t="n">
+        <f aca="false">(E8-J8-G8) * D8</f>
+        <v>20.69</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="0" t="s">
         <v>23</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>22</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>1</v>
@@ -618,21 +1277,25 @@
         <v>55.69</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J9" s="0" t="n">
         <v>27.29</v>
       </c>
+      <c r="K9" s="0" t="n">
+        <f aca="false">(E9-J9-G9) * D9</f>
+        <v>17.71</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>1</v>
@@ -650,21 +1313,25 @@
         <v>74.25</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J10" s="0" t="n">
         <v>45.29</v>
       </c>
+      <c r="K10" s="0" t="n">
+        <f aca="false">(E10-J10-G10) * D10</f>
+        <v>14.71</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>1</v>
@@ -682,21 +1349,25 @@
         <v>55.69</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J11" s="0" t="n">
         <v>27.29</v>
       </c>
+      <c r="K11" s="0" t="n">
+        <f aca="false">(E11-J11-G11) * D11</f>
+        <v>17.71</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>1</v>
@@ -714,21 +1385,25 @@
         <v>117.56</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J12" s="0" t="n">
         <v>43.5</v>
       </c>
+      <c r="K12" s="0" t="n">
+        <f aca="false">(E12-J12-G12) * D12</f>
+        <v>51.5</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>1</v>
@@ -746,21 +1421,25 @@
         <v>142.31</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J13" s="0" t="n">
         <v>68.31</v>
       </c>
+      <c r="K13" s="0" t="n">
+        <f aca="false">(E13-J13-G13) * D13</f>
+        <v>46.69</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>1</v>
@@ -778,21 +1457,25 @@
         <v>105.19</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J14" s="0" t="n">
         <v>31.56</v>
       </c>
+      <c r="K14" s="0" t="n">
+        <f aca="false">(E14-J14-G14) * D14</f>
+        <v>53.44</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>1</v>
@@ -810,21 +1493,25 @@
         <v>105.19</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J15" s="0" t="n">
         <v>66.27</v>
       </c>
+      <c r="K15" s="0" t="n">
+        <f aca="false">(E15-J15-G15) * D15</f>
+        <v>18.73</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="0" t="s">
         <v>35</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>34</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>2</v>
@@ -842,21 +1529,25 @@
         <v>210.38</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J16" s="0" t="n">
         <v>31.56</v>
       </c>
+      <c r="K16" s="0" t="n">
+        <f aca="false">(E16-J16-G16) * D16</f>
+        <v>106.88</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>1</v>
@@ -874,21 +1565,25 @@
         <v>74.25</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J17" s="0" t="n">
         <v>45.29</v>
       </c>
+      <c r="K17" s="0" t="n">
+        <f aca="false">(E17-J17-G17) * D17</f>
+        <v>14.71</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>1</v>
@@ -906,21 +1601,25 @@
         <v>61.88</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J18" s="0" t="n">
         <v>31.56</v>
       </c>
+      <c r="K18" s="0" t="n">
+        <f aca="false">(E18-J18-G18) * D18</f>
+        <v>18.44</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>2</v>
@@ -938,21 +1637,25 @@
         <v>148.5</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J19" s="0" t="n">
         <v>45.29</v>
       </c>
+      <c r="K19" s="0" t="n">
+        <f aca="false">(E19-J19-G19) * D19</f>
+        <v>29.42</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>1</v>
@@ -970,21 +1673,25 @@
         <v>61.88</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J20" s="0" t="n">
         <v>31.56</v>
       </c>
+      <c r="K20" s="0" t="n">
+        <f aca="false">(E20-J20-G20) * D20</f>
+        <v>18.44</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>1</v>
@@ -1002,15 +1709,19 @@
         <v>105.19</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J21" s="0" t="n">
         <v>48.39</v>
       </c>
+      <c r="K21" s="0" t="n">
+        <f aca="false">(E21-J21-G21) * D21</f>
+        <v>36.61</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1018,18 +1729,18 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B27" s="0" t="n">
         <f aca="false">SUMPRODUCT(E2:E21, D2:D21) + SUM(F2:F21) - SUM(G2:G21)</f>
@@ -1042,7 +1753,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B28" s="0" t="n">
         <f aca="false">SUMPRODUCT(J2:J21, D2:D21)</f>
@@ -1055,7 +1766,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B29" s="0" t="n">
         <f aca="false">SUMPRODUCT((E2:E21 - J2:J21 - G2:G21) * D2:D21)</f>
@@ -1068,7 +1779,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B30" s="0" t="n">
         <f aca="false">(B29/B27) * 100</f>
@@ -1081,7 +1792,7 @@
     </row>
     <row r="31" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B31" s="0" t="n">
         <f aca="false">B27</f>
@@ -1090,6 +1801,128 @@
       <c r="C31" s="3" t="b">
         <f aca="false">1782.04=B31</f>
         <v>1</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35" s="10" t="n">
+        <v>46.69</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C36" s="12" t="n">
+        <v>58.84</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" s="12" t="n">
+        <v>18.73</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C38" s="12" t="n">
+        <v>160.32</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C39" s="12" t="n">
+        <v>41.38</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C40" s="12" t="n">
+        <v>36.61</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C41" s="12" t="n">
+        <v>24.51</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C42" s="12" t="n">
+        <v>53.13</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43" s="12" t="n">
+        <v>92.2</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C44" s="13" t="n">
+        <v>51.5</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C45" s="15" t="n">
+        <v>583.91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>